<commit_message>
Excel Update, Zeiten verändert
</commit_message>
<xml_diff>
--- a/datein/Test.xlsx
+++ b/datein/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\GitHub\koord-app-altenberge\datein\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67431945-4E91-4A60-8F45-88B24544740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E95C12-AB6D-4625-AEC4-5C7E63EB16FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schueler" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="125">
   <si>
     <t>vorname</t>
   </si>
@@ -240,9 +240,6 @@
     <t>sophiemusterfrau</t>
   </si>
   <si>
-    <t>Mensa</t>
-  </si>
-  <si>
     <t>Computerraum</t>
   </si>
   <si>
@@ -406,6 +403,18 @@
   </si>
   <si>
     <t>2C</t>
+  </si>
+  <si>
+    <t>Mensa 1</t>
+  </si>
+  <si>
+    <t>Mensa 2</t>
+  </si>
+  <si>
+    <t>Mensa 3</t>
+  </si>
+  <si>
+    <t>Aushilfskraft</t>
   </si>
 </sst>
 </file>
@@ -782,17 +791,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.81640625" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -838,7 +847,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -861,7 +870,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -884,7 +893,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -907,9 +916,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -930,9 +939,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -953,9 +962,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -976,9 +985,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -987,7 +996,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -999,9 +1008,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -1022,9 +1031,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -1033,7 +1042,7 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -1045,9 +1054,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1056,7 +1065,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1068,9 +1077,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1079,7 +1088,7 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
@@ -1091,18 +1100,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -1114,18 +1123,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
@@ -1137,18 +1146,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -1160,18 +1169,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -1183,18 +1192,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -1206,18 +1215,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -1229,9 +1238,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -1240,7 +1249,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -1252,9 +1261,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
@@ -1263,7 +1272,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -1275,9 +1284,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1286,7 +1295,7 @@
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -1298,9 +1307,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -1321,18 +1330,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -1344,18 +1353,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1367,18 +1376,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -1390,18 +1399,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -1413,18 +1422,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -1436,9 +1445,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -1459,9 +1468,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
@@ -1470,7 +1479,7 @@
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1482,9 +1491,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
@@ -1505,9 +1514,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1516,7 +1525,7 @@
         <v>19</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
@@ -1528,9 +1537,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -1539,7 +1548,7 @@
         <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
@@ -1551,18 +1560,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" t="s">
         <v>16</v>
@@ -1574,18 +1583,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
@@ -1597,15 +1606,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" t="s">
         <v>38</v>
@@ -1620,15 +1629,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37" t="s">
         <v>38</v>
@@ -1666,19 +1675,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1720,7 +1729,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1734,9 +1743,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1748,9 +1757,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -1762,9 +1771,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -1776,9 +1785,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1787,6 +1796,76 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1804,15 +1883,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" customWidth="1"/>
-    <col min="11" max="11" width="20.26953125" customWidth="1"/>
-    <col min="12" max="12" width="16.1796875" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1850,7 +1929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1882,7 +1961,7 @@
         <v>45337</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1921,14 +2000,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1939,7 +2018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1950,48 +2029,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2001,15 +2080,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C266C4C-9DC7-429B-B311-1310086F7055}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2020,7 +2099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2031,7 +2110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -2042,7 +2121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -2053,7 +2132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2064,9 +2143,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2075,9 +2154,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2086,9 +2165,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2097,9 +2176,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2108,7 +2187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>302</v>
       </c>
@@ -2117,6 +2196,28 @@
       </c>
       <c r="C10">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>